<commit_message>
OO14_ProcessTest_with_inputs_and_outputs_modify wo checking yet (test cases 21-32).
</commit_message>
<xml_diff>
--- a/soberano/test_cases/worker_modify_test_cases.xlsx
+++ b/soberano/test_cases/worker_modify_test_cases.xlsx
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Procurement worker, Salesclerk, Shift manager</t>
   </si>
   <si>
-    <t xml:space="preserve">user10 can not even list the users</t>
+    <t xml:space="preserve">user10 is NOT allowed to modify a user, but it can list the users</t>
   </si>
   <si>
     <t xml:space="preserve">Procurement worker, Salesclerk</t>
@@ -372,13 +372,13 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A12" activeCellId="0" sqref="12:12"/>
+      <selection pane="topRight" activeCell="A13" activeCellId="0" sqref="13:13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.92"/>
@@ -390,7 +390,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="10.32"/>

</xml_diff>